<commit_message>
Fixing the code and making it more structural
</commit_message>
<xml_diff>
--- a/Data/data.xlsx
+++ b/Data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x496784\Downloads\NedBank_Assessment2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB331762\Music\AUTOMATION\Git\iLab Quality\Absa_Assessment\Absa_Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C55961-F562-4708-8C20-CBFB92BEA565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DA33B7-2D61-45B3-B447-CE98895A8F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{0397E3FF-0163-4BAE-9A54-145CB4ACB2A3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0397E3FF-0163-4BAE-9A54-145CB4ACB2A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -38,16 +38,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Username</t>
+    <t>http://www.way2automation.com/angularjs-protractor/webtables/</t>
   </si>
   <si>
-    <t>Password</t>
+    <t>url</t>
   </si>
   <si>
-    <t>Password01!</t>
+    <t>browser</t>
   </si>
   <si>
-    <t>test</t>
+    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -71,7 +71,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,17 +96,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -121,9 +125,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -161,7 +165,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -267,7 +271,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -409,7 +413,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -420,7 +424,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,10 +434,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -441,12 +445,15 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{19C54E11-F66A-45AA-97F0-C774BC484C67}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>